<commit_message>
Before disturbing closeness function
</commit_message>
<xml_diff>
--- a/drl/computational/policy_irrational_delta prob 10.xlsx
+++ b/drl/computational/policy_irrational_delta prob 10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Semester 1 2020\COMP90055\DRL-Policy-Gradient\drl\computational\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BABF84A-CB46-43D2-9C53-E539E406DDAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E160F959-F1D4-4D89-8CD0-A964067E430A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3251" uniqueCount="87">
   <si>
     <t>map</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Sum of Deceptive</t>
-  </si>
-  <si>
-    <t>Sum of Deceptive2</t>
   </si>
   <si>
     <t>Count of Deceptive2</t>
@@ -1544,228 +1541,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sum of Deceptive2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$4:$A$34</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="27"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>D_10</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>D_20</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>D_30</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>D_40</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>D_50</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>D_60</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>D_70</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>D_80</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>D_90</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>D_10</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>D_20</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>D_30</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>D_40</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>D_50</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>D_60</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>D_70</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>D_80</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>D_90</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>D_10</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>D_20</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>D_30</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>D_40</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>D_50</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>D_60</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>D_70</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>D_80</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>D_90</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>49_high</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>49_low</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>empty</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F749-4C98-AD45-8A8E07F8F548}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -12391,7 +12166,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F8F877C3-02E7-4E21-B578-028E5334C13D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:D34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:C34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="22">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -12538,23 +12313,19 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
   </colItems>
-  <dataFields count="3">
+  <dataFields count="2">
     <dataField name="Sum of Deceptive" fld="21" baseField="0" baseItem="0"/>
     <dataField name="Count of Deceptive2" fld="21" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Deceptive2" fld="21" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="2">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -12569,15 +12340,6 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -12892,10 +12654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B1EBDF-97D9-425C-906D-34CD69FBCD3B}">
-  <dimension ref="A3:D34"/>
+  <dimension ref="A3:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12906,7 +12668,7 @@
     <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -12914,13 +12676,10 @@
         <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
@@ -12930,11 +12689,8 @@
       <c r="C4" s="4">
         <v>72</v>
       </c>
-      <c r="D4" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -12944,11 +12700,8 @@
       <c r="C5" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -12958,11 +12711,8 @@
       <c r="C6" s="4">
         <v>8</v>
       </c>
-      <c r="D6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -12972,11 +12722,8 @@
       <c r="C7" s="4">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -12986,11 +12733,8 @@
       <c r="C8" s="4">
         <v>8</v>
       </c>
-      <c r="D8" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -13000,11 +12744,8 @@
       <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -13014,11 +12755,8 @@
       <c r="C10" s="4">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -13028,11 +12766,8 @@
       <c r="C11" s="4">
         <v>8</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -13042,11 +12777,8 @@
       <c r="C12" s="4">
         <v>8</v>
       </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -13056,11 +12788,8 @@
       <c r="C13" s="4">
         <v>8</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -13070,11 +12799,8 @@
       <c r="C14" s="4">
         <v>84</v>
       </c>
-      <c r="D14" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -13084,11 +12810,8 @@
       <c r="C15" s="4">
         <v>10</v>
       </c>
-      <c r="D15" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -13098,11 +12821,8 @@
       <c r="C16" s="4">
         <v>10</v>
       </c>
-      <c r="D16" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -13112,11 +12832,8 @@
       <c r="C17" s="4">
         <v>10</v>
       </c>
-      <c r="D17" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -13126,11 +12843,8 @@
       <c r="C18" s="4">
         <v>10</v>
       </c>
-      <c r="D18" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
@@ -13140,11 +12854,8 @@
       <c r="C19" s="4">
         <v>10</v>
       </c>
-      <c r="D19" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -13154,11 +12865,8 @@
       <c r="C20" s="4">
         <v>9</v>
       </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
@@ -13168,11 +12876,8 @@
       <c r="C21" s="4">
         <v>9</v>
       </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -13182,11 +12887,8 @@
       <c r="C22" s="4">
         <v>8</v>
       </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -13196,11 +12898,8 @@
       <c r="C23" s="4">
         <v>8</v>
       </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
@@ -13210,11 +12909,8 @@
       <c r="C24" s="4">
         <v>249</v>
       </c>
-      <c r="D24" s="4">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
@@ -13224,11 +12920,8 @@
       <c r="C25" s="4">
         <v>28</v>
       </c>
-      <c r="D25" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
@@ -13238,11 +12931,8 @@
       <c r="C26" s="4">
         <v>28</v>
       </c>
-      <c r="D26" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -13252,11 +12942,8 @@
       <c r="C27" s="4">
         <v>28</v>
       </c>
-      <c r="D27" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
@@ -13266,11 +12953,8 @@
       <c r="C28" s="4">
         <v>28</v>
       </c>
-      <c r="D28" s="4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
@@ -13280,11 +12964,8 @@
       <c r="C29" s="4">
         <v>28</v>
       </c>
-      <c r="D29" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
@@ -13294,11 +12975,8 @@
       <c r="C30" s="4">
         <v>28</v>
       </c>
-      <c r="D30" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -13308,11 +12986,8 @@
       <c r="C31" s="4">
         <v>27</v>
       </c>
-      <c r="D31" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>26</v>
       </c>
@@ -13322,11 +12997,8 @@
       <c r="C32" s="4">
         <v>27</v>
       </c>
-      <c r="D32" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>27</v>
       </c>
@@ -13336,11 +13008,8 @@
       <c r="C33" s="4">
         <v>27</v>
       </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>83</v>
       </c>
@@ -13349,9 +13018,6 @@
       </c>
       <c r="C34" s="4">
         <v>405</v>
-      </c>
-      <c r="D34" s="4">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>